<commit_message>
modifid the linux graph
</commit_message>
<xml_diff>
--- a/result_graphs/npb-benchmark-total-t4-linux.xlsx
+++ b/result_graphs/npb-benchmark-total-t4-linux.xlsx
@@ -5,11 +5,11 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itomaldonado/git/multiprocessor-benchmarking-exploration/Graphed Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itomaldonado/git/multiprocessor-benchmarking-exploration/result_graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="npb-benchmark-total-output" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="77" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -767,11 +767,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2054259712"/>
-        <c:axId val="-1187939392"/>
+        <c:axId val="2127533280"/>
+        <c:axId val="2127536896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2054259712"/>
+        <c:axId val="2127533280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +842,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1187939392"/>
+        <c:crossAx val="2127536896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -850,7 +850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1187939392"/>
+        <c:axId val="2127536896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,7 +901,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2054259712"/>
+        <c:crossAx val="2127533280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1483,11 +1483,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2122470208"/>
-        <c:axId val="-2051275712"/>
+        <c:axId val="2127194544"/>
+        <c:axId val="2127198160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2122470208"/>
+        <c:axId val="2127194544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1558,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2051275712"/>
+        <c:crossAx val="2127198160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1566,7 +1566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2051275712"/>
+        <c:axId val="2127198160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1617,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122470208"/>
+        <c:crossAx val="2127194544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2222,11 +2222,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109610288"/>
-        <c:axId val="-1027101968"/>
+        <c:axId val="-2137041216"/>
+        <c:axId val="-2137037600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2109610288"/>
+        <c:axId val="-2137041216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2297,7 +2297,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1027101968"/>
+        <c:crossAx val="-2137037600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2305,7 +2305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1027101968"/>
+        <c:axId val="-2137037600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2356,7 +2356,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2109610288"/>
+        <c:crossAx val="-2137041216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2681,14 +2681,14 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Chart-Data'!$H$43:$I$43</c:f>
+              <c:f>'Chart-Data'!$H$42:$I$42</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>MG</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>S</c:v>
+                  <c:v>C</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2739,7 +2739,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart-Data'!$J$43:$M$43</c:f>
+              <c:f>'Chart-Data'!$J$42:$M$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2747,13 +2747,13 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2</c:v>
+                  <c:v>1.177752288576525</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2</c:v>
+                  <c:v>1.1615417370995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2</c:v>
+                  <c:v>1.162757052805621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2765,14 +2765,14 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Chart-Data'!$H$44:$I$44</c:f>
+              <c:f>'Chart-Data'!$H$43:$I$43</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>MG</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>W</c:v>
+                  <c:v>S</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2823,7 +2823,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart-Data'!$J$44:$M$44</c:f>
+              <c:f>'Chart-Data'!$J$43:$M$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2831,13 +2831,13 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.410472972972973</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.444636678200692</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.434707903780069</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2849,14 +2849,14 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Chart-Data'!$H$42:$I$42</c:f>
+              <c:f>'Chart-Data'!$H$44:$I$44</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>MG</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>C</c:v>
+                  <c:v>W</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2907,7 +2907,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Chart-Data'!$J$42:$M$42</c:f>
+              <c:f>'Chart-Data'!$J$44:$M$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -2915,13 +2915,13 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.177752288576525</c:v>
+                  <c:v>1.410472972972973</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1615417370995</c:v>
+                  <c:v>1.444636678200692</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.162757052805621</c:v>
+                  <c:v>1.434707903780069</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2938,11 +2938,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2084875024"/>
-        <c:axId val="-2035503664"/>
+        <c:axId val="-2137226704"/>
+        <c:axId val="-2137223088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2084875024"/>
+        <c:axId val="-2137226704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3013,7 +3013,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2035503664"/>
+        <c:crossAx val="-2137223088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3021,7 +3021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2035503664"/>
+        <c:axId val="-2137223088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3072,7 +3072,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2084875024"/>
+        <c:crossAx val="-2137226704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3654,11 +3654,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2050044928"/>
-        <c:axId val="-2130393088"/>
+        <c:axId val="2127069872"/>
+        <c:axId val="2127073488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2050044928"/>
+        <c:axId val="2127069872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3729,7 +3729,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130393088"/>
+        <c:crossAx val="2127073488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3737,7 +3737,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130393088"/>
+        <c:axId val="2127073488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3788,7 +3788,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2050044928"/>
+        <c:crossAx val="2127069872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4388,11 +4388,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2050973440"/>
-        <c:axId val="-2037675488"/>
+        <c:axId val="2126991488"/>
+        <c:axId val="2126995104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2050973440"/>
+        <c:axId val="2126991488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4463,7 +4463,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2037675488"/>
+        <c:crossAx val="2126995104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4471,7 +4471,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2037675488"/>
+        <c:axId val="2126995104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4522,7 +4522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2050973440"/>
+        <c:crossAx val="2126991488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5104,11 +5104,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2039042032"/>
-        <c:axId val="-2050924864"/>
+        <c:axId val="-2137350848"/>
+        <c:axId val="-2137347232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2039042032"/>
+        <c:axId val="-2137350848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5179,7 +5179,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2050924864"/>
+        <c:crossAx val="-2137347232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5187,7 +5187,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2050924864"/>
+        <c:axId val="-2137347232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5238,7 +5238,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2039042032"/>
+        <c:crossAx val="-2137350848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5820,11 +5820,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-922998944"/>
-        <c:axId val="-2040340528"/>
+        <c:axId val="2126948064"/>
+        <c:axId val="2126935344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-922998944"/>
+        <c:axId val="2126948064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5895,7 +5895,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2040340528"/>
+        <c:crossAx val="2126935344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5903,7 +5903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2040340528"/>
+        <c:axId val="2126935344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5954,7 +5954,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-922998944"/>
+        <c:crossAx val="2126948064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10455,7 +10455,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -16331,7 +16331,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NPB-Run-Time" cacheId="77" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NPB-Run-Time" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="A3:F52" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -31381,8 +31381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added presentation, modified readme to reflect changes, finalized graphs and results.
</commit_message>
<xml_diff>
--- a/result_graphs/npb-benchmark-total-t4-linux.xlsx
+++ b/result_graphs/npb-benchmark-total-t4-linux.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="npb-benchmark-total-output" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId12"/>
+    <pivotCache cacheId="29" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -767,11 +767,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127533280"/>
-        <c:axId val="2127536896"/>
+        <c:axId val="-2122686896"/>
+        <c:axId val="-2122753408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127533280"/>
+        <c:axId val="-2122686896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -842,7 +842,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127536896"/>
+        <c:crossAx val="-2122753408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -850,7 +850,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127536896"/>
+        <c:axId val="-2122753408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -901,7 +901,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127533280"/>
+        <c:crossAx val="-2122686896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1017,7 +1017,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1483,11 +1482,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127194544"/>
-        <c:axId val="2127198160"/>
+        <c:axId val="-2122788720"/>
+        <c:axId val="-2122831072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127194544"/>
+        <c:axId val="-2122788720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1557,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127198160"/>
+        <c:crossAx val="-2122831072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1566,7 +1565,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127198160"/>
+        <c:axId val="-2122831072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1616,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127194544"/>
+        <c:crossAx val="-2122788720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1654,7 +1653,6 @@
           </a:p>
         </c:txPr>
       </c:legendEntry>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1756,7 +1754,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2222,11 +2219,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2137041216"/>
-        <c:axId val="-2137037600"/>
+        <c:axId val="-2113314736"/>
+        <c:axId val="-2053310640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2137041216"/>
+        <c:axId val="-2113314736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2297,7 +2294,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2137037600"/>
+        <c:crossAx val="-2053310640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2305,7 +2302,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137037600"/>
+        <c:axId val="-2053310640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2356,7 +2353,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2137041216"/>
+        <c:crossAx val="-2113314736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2370,7 +2367,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2472,7 +2468,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2938,11 +2933,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2137226704"/>
-        <c:axId val="-2137223088"/>
+        <c:axId val="2077406640"/>
+        <c:axId val="1822493392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2137226704"/>
+        <c:axId val="2077406640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3013,7 +3008,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2137223088"/>
+        <c:crossAx val="1822493392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3021,7 +3016,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137223088"/>
+        <c:axId val="1822493392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3072,7 +3067,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2137226704"/>
+        <c:crossAx val="2077406640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3086,7 +3081,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3188,7 +3182,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3654,11 +3647,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2127069872"/>
-        <c:axId val="2127073488"/>
+        <c:axId val="-2055083312"/>
+        <c:axId val="-2110657168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2127069872"/>
+        <c:axId val="-2055083312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3729,7 +3722,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127073488"/>
+        <c:crossAx val="-2110657168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3737,7 +3730,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127073488"/>
+        <c:axId val="-2110657168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3788,7 +3781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127069872"/>
+        <c:crossAx val="-2055083312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3802,7 +3795,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3912,7 +3904,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4388,11 +4379,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126991488"/>
-        <c:axId val="2126995104"/>
+        <c:axId val="-2107121216"/>
+        <c:axId val="-2050108672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126991488"/>
+        <c:axId val="-2107121216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4463,7 +4454,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126995104"/>
+        <c:crossAx val="-2050108672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4471,7 +4462,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126995104"/>
+        <c:axId val="-2050108672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4522,7 +4513,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126991488"/>
+        <c:crossAx val="-2107121216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4536,7 +4527,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4638,7 +4628,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5104,11 +5093,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2137350848"/>
-        <c:axId val="-2137347232"/>
+        <c:axId val="-2106962256"/>
+        <c:axId val="2110949296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2137350848"/>
+        <c:axId val="-2106962256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5179,7 +5168,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2137347232"/>
+        <c:crossAx val="2110949296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5187,7 +5176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2137347232"/>
+        <c:axId val="2110949296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5238,7 +5227,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2137350848"/>
+        <c:crossAx val="-2106962256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5252,7 +5241,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5354,7 +5342,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5820,11 +5807,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126948064"/>
-        <c:axId val="2126935344"/>
+        <c:axId val="-2052897504"/>
+        <c:axId val="-2054388448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126948064"/>
+        <c:axId val="-2052897504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5895,7 +5882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126935344"/>
+        <c:crossAx val="-2054388448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5903,7 +5890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126935344"/>
+        <c:axId val="-2054388448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5954,7 +5941,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126948064"/>
+        <c:crossAx val="-2052897504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5968,7 +5955,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -16331,7 +16317,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NPB-Run-Time" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="NPB-Run-Time" cacheId="29" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="A3:F52" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -16841,9 +16827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E800"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -31381,7 +31365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>

</xml_diff>